<commit_message>
Update pages with new guide details.
</commit_message>
<xml_diff>
--- a/input/images/ICSR_Field_Listing_and_FHIR_Mapping.xlsx
+++ b/input/images/ICSR_Field_Listing_and_FHIR_Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeanduteau/Documents/DDIWork/IBM-BEST/fhir-icsr-ae-reporting/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4BE254-291F-BA4D-BF1A-99944F2FB042}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C977DEC0-74B7-F443-AA40-4F1E1F86FD09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26780" windowHeight="27700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11100" yWindow="28800" windowWidth="26780" windowHeight="19420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICSR FIELDS" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6534" uniqueCount="1958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6511" uniqueCount="1955">
   <si>
     <t>CONF</t>
   </si>
@@ -5984,9 +5984,6 @@
     <t>FDA CBER BEST Automated AE Reporting Prototype Case</t>
   </si>
   <si>
-    <t>Hardcode</t>
-  </si>
-  <si>
     <t>B.5.1 LINE 2</t>
   </si>
   <si>
@@ -6005,9 +6002,6 @@
     <t>Definitive</t>
   </si>
   <si>
-    <t>BEST clinical assessment</t>
-  </si>
-  <si>
     <t>B.5.1 LINE 4</t>
   </si>
   <si>
@@ -6026,9 +6020,6 @@
     <t>Probable</t>
   </si>
   <si>
-    <t>BEST clinical assessment (somewhat similar to B.4.k.1)</t>
-  </si>
-  <si>
     <t>B.5.1 LINE 6</t>
   </si>
   <si>
@@ -6095,9 +6086,6 @@
     <t>&lt;PATIENT BLOOD GROUP&gt;</t>
   </si>
   <si>
-    <t>Automated population</t>
-  </si>
-  <si>
     <t>B.5.1 LINE 15</t>
   </si>
   <si>
@@ -6167,9 +6155,6 @@
     <t>&lt;INSERT BEST CLINICAL REVIEWER CASE NARRATIVE&gt;</t>
   </si>
   <si>
-    <t>Varies by phenotype.</t>
-  </si>
-  <si>
     <t>H.1 CASE NARRATIVE RETURN DELIMITED LINES</t>
   </si>
   <si>
@@ -6198,6 +6183,12 @@
   </si>
   <si>
     <t>H.1 LINE 7</t>
+  </si>
+  <si>
+    <t>CASE NARRATIVE FIELD</t>
+  </si>
+  <si>
+    <t>SAMPLE DATA</t>
   </si>
 </sst>
 </file>
@@ -6728,7 +6719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F243" workbookViewId="0">
+    <sheetView topLeftCell="F243" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -26108,10 +26099,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64062B5B-6E9E-B649-A773-97A21E2861DA}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26119,447 +26110,375 @@
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>1953</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="62" t="s">
         <v>1881</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="62" t="s">
+      <c r="B2" s="63"/>
+      <c r="C2" s="62" t="s">
         <v>1882</v>
       </c>
-      <c r="E1" s="64"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="65" t="s">
+      <c r="D2" s="64"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="65" t="s">
         <v>1883</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B3" s="65" t="s">
         <v>1884</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C3" s="66" t="s">
         <v>1885</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="D3" s="67"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="65" t="s">
         <v>1886</v>
       </c>
-      <c r="E2" s="67"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="65" t="s">
+      <c r="B4" s="65" t="s">
         <v>1887</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="C4" s="66" t="s">
         <v>1888</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="D4" s="67"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="65" t="s">
         <v>1889</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="B5" s="65" t="s">
+        <v>1890</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>1891</v>
+      </c>
+      <c r="D5" s="67"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="65" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B6" s="65" t="s">
+        <v>1893</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>1894</v>
+      </c>
+      <c r="D6" s="67"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="65" t="s">
+        <v>1895</v>
+      </c>
+      <c r="B7" s="65" t="s">
+        <v>1896</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>1897</v>
+      </c>
+      <c r="D7" s="67"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="65" t="s">
+        <v>1898</v>
+      </c>
+      <c r="B8" s="65" t="s">
+        <v>1899</v>
+      </c>
+      <c r="C8" s="66">
+        <v>3500</v>
+      </c>
+      <c r="D8" s="67"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="65" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B9" s="65" t="s">
+        <v>1901</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>1902</v>
+      </c>
+      <c r="D9" s="67"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="65" t="s">
+        <v>1903</v>
+      </c>
+      <c r="B10" s="65" t="s">
+        <v>1904</v>
+      </c>
+      <c r="C10" s="66">
+        <v>1</v>
+      </c>
+      <c r="D10" s="67"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="65" t="s">
+        <v>1905</v>
+      </c>
+      <c r="B11" s="65" t="s">
+        <v>1906</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>1907</v>
+      </c>
+      <c r="D11" s="67"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="65" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B12" s="65" t="s">
+        <v>1909</v>
+      </c>
+      <c r="C12" s="66" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="67"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="65" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B13" s="65" t="s">
+        <v>1911</v>
+      </c>
+      <c r="C13" s="66">
+        <v>1</v>
+      </c>
+      <c r="D13" s="67"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="65" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>1913</v>
+      </c>
+      <c r="C14" s="66">
+        <v>2</v>
+      </c>
+      <c r="D14" s="67"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="65" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B15" s="65" t="s">
+        <v>1915</v>
+      </c>
+      <c r="C15" s="66" t="s">
+        <v>1916</v>
+      </c>
+      <c r="D15" s="67"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="65" t="s">
+        <v>1917</v>
+      </c>
+      <c r="B16" s="65" t="s">
+        <v>1918</v>
+      </c>
+      <c r="C16" s="66" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D16" s="67"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="65" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B17" s="65" t="s">
+        <v>1921</v>
+      </c>
+      <c r="C17" s="66" t="s">
+        <v>1922</v>
+      </c>
+      <c r="D17" s="67"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="65" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B18" s="65" t="s">
+        <v>1924</v>
+      </c>
+      <c r="C18" s="66" t="s">
+        <v>1925</v>
+      </c>
+      <c r="D18" s="67"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="65" t="s">
+        <v>1926</v>
+      </c>
+      <c r="B19" s="65" t="s">
+        <v>1927</v>
+      </c>
+      <c r="C19" s="66" t="s">
+        <v>1928</v>
+      </c>
+      <c r="D19" s="67"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="65" t="s">
+        <v>1929</v>
+      </c>
+      <c r="B20" s="65" t="s">
+        <v>1930</v>
+      </c>
+      <c r="C20" s="66" t="s">
+        <v>1931</v>
+      </c>
+      <c r="D20" s="67"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="65" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B21" s="65" t="s">
+        <v>1933</v>
+      </c>
+      <c r="C21" s="66">
+        <v>2</v>
+      </c>
+      <c r="D21" s="67"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="65" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B22" s="65" t="s">
+        <v>1935</v>
+      </c>
+      <c r="C22" s="66" t="s">
+        <v>1936</v>
+      </c>
+      <c r="D22" s="67"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="65" t="s">
+        <v>1937</v>
+      </c>
+      <c r="B23" s="65" t="s">
+        <v>1938</v>
+      </c>
+      <c r="C23" s="66" t="s">
+        <v>1939</v>
+      </c>
+      <c r="D23" s="67"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="65" t="s">
+        <v>1940</v>
+      </c>
+      <c r="B24" s="65" t="s">
+        <v>1941</v>
+      </c>
+      <c r="C24" s="66" t="s">
+        <v>1942</v>
+      </c>
+      <c r="D24" s="67"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="62" t="s">
+        <v>1943</v>
+      </c>
+      <c r="B26" s="63"/>
+      <c r="C26" s="62" t="s">
+        <v>1882</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="65" t="s">
+        <v>1944</v>
+      </c>
+      <c r="B27" s="65" t="s">
+        <v>1884</v>
+      </c>
+      <c r="C27" s="66" t="s">
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="65" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B28" s="65" t="s">
+        <v>1887</v>
+      </c>
+      <c r="C28" s="66" t="s">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="65" t="s">
         <v>1947</v>
       </c>
-      <c r="E3" s="67"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="65" t="s">
+      <c r="B29" s="65" t="s">
         <v>1890</v>
       </c>
-      <c r="B4" s="65" t="s">
+      <c r="C29" s="66" t="s">
         <v>1891</v>
       </c>
-      <c r="C4" s="66" t="s">
-        <v>1892</v>
-      </c>
-      <c r="D4" s="65" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="65" t="s">
+        <v>1948</v>
+      </c>
+      <c r="B30" s="65" t="s">
         <v>1893</v>
       </c>
-      <c r="E4" s="67"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="65" t="s">
+      <c r="C30" s="66" t="s">
         <v>1894</v>
       </c>
-      <c r="B5" s="65" t="s">
-        <v>1895</v>
-      </c>
-      <c r="C5" s="66" t="s">
-        <v>1896</v>
-      </c>
-      <c r="D5" s="65" t="s">
-        <v>1893</v>
-      </c>
-      <c r="E5" s="67"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="65" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="65" t="s">
+        <v>1949</v>
+      </c>
+      <c r="B31" s="65" t="s">
+        <v>1950</v>
+      </c>
+      <c r="C31" s="66" t="s">
         <v>1897</v>
       </c>
-      <c r="B6" s="65" t="s">
-        <v>1898</v>
-      </c>
-      <c r="C6" s="66" t="s">
-        <v>1899</v>
-      </c>
-      <c r="D6" s="65" t="s">
-        <v>1900</v>
-      </c>
-      <c r="E6" s="67"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="65" t="s">
-        <v>1901</v>
-      </c>
-      <c r="B7" s="65" t="s">
-        <v>1902</v>
-      </c>
-      <c r="C7" s="66">
-        <v>3500</v>
-      </c>
-      <c r="D7" s="65" t="s">
-        <v>1886</v>
-      </c>
-      <c r="E7" s="67"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="65" t="s">
-        <v>1903</v>
-      </c>
-      <c r="B8" s="65" t="s">
-        <v>1904</v>
-      </c>
-      <c r="C8" s="66" t="s">
-        <v>1905</v>
-      </c>
-      <c r="D8" s="65" t="s">
-        <v>1886</v>
-      </c>
-      <c r="E8" s="67"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="65" t="s">
-        <v>1906</v>
-      </c>
-      <c r="B9" s="65" t="s">
-        <v>1907</v>
-      </c>
-      <c r="C9" s="66">
-        <v>1</v>
-      </c>
-      <c r="D9" s="65" t="s">
-        <v>1886</v>
-      </c>
-      <c r="E9" s="67"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="65" t="s">
-        <v>1908</v>
-      </c>
-      <c r="B10" s="65" t="s">
-        <v>1909</v>
-      </c>
-      <c r="C10" s="66" t="s">
-        <v>1910</v>
-      </c>
-      <c r="D10" s="65" t="s">
-        <v>1886</v>
-      </c>
-      <c r="E10" s="67"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="65" t="s">
-        <v>1911</v>
-      </c>
-      <c r="B11" s="65" t="s">
-        <v>1912</v>
-      </c>
-      <c r="C11" s="66" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="65" t="s">
-        <v>1886</v>
-      </c>
-      <c r="E11" s="67"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="65" t="s">
-        <v>1913</v>
-      </c>
-      <c r="B12" s="65" t="s">
-        <v>1914</v>
-      </c>
-      <c r="C12" s="66">
-        <v>1</v>
-      </c>
-      <c r="D12" s="65" t="s">
-        <v>1886</v>
-      </c>
-      <c r="E12" s="67"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="65" t="s">
-        <v>1915</v>
-      </c>
-      <c r="B13" s="65" t="s">
-        <v>1916</v>
-      </c>
-      <c r="C13" s="66">
-        <v>2</v>
-      </c>
-      <c r="D13" s="65" t="s">
-        <v>1886</v>
-      </c>
-      <c r="E13" s="67"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="65" t="s">
-        <v>1917</v>
-      </c>
-      <c r="B14" s="65" t="s">
-        <v>1918</v>
-      </c>
-      <c r="C14" s="66" t="s">
-        <v>1919</v>
-      </c>
-      <c r="D14" s="65" t="s">
-        <v>1886</v>
-      </c>
-      <c r="E14" s="67"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="65" t="s">
-        <v>1920</v>
-      </c>
-      <c r="B15" s="65" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="65" t="s">
+        <v>1951</v>
+      </c>
+      <c r="B32" s="65" t="s">
         <v>1921</v>
       </c>
-      <c r="C15" s="66" t="s">
+      <c r="C32" s="66" t="s">
         <v>1922</v>
       </c>
-      <c r="D15" s="65" t="s">
-        <v>1923</v>
-      </c>
-      <c r="E15" s="67"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="65" t="s">
-        <v>1924</v>
-      </c>
-      <c r="B16" s="65" t="s">
-        <v>1925</v>
-      </c>
-      <c r="C16" s="66" t="s">
-        <v>1926</v>
-      </c>
-      <c r="D16" s="65" t="s">
-        <v>1886</v>
-      </c>
-      <c r="E16" s="67"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="65" t="s">
-        <v>1927</v>
-      </c>
-      <c r="B17" s="65" t="s">
-        <v>1928</v>
-      </c>
-      <c r="C17" s="66" t="s">
-        <v>1929</v>
-      </c>
-      <c r="D17" s="65" t="s">
-        <v>1923</v>
-      </c>
-      <c r="E17" s="67"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="65" t="s">
-        <v>1930</v>
-      </c>
-      <c r="B18" s="65" t="s">
-        <v>1931</v>
-      </c>
-      <c r="C18" s="66" t="s">
-        <v>1932</v>
-      </c>
-      <c r="D18" s="65" t="s">
-        <v>1923</v>
-      </c>
-      <c r="E18" s="67"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="65" t="s">
-        <v>1933</v>
-      </c>
-      <c r="B19" s="65" t="s">
-        <v>1934</v>
-      </c>
-      <c r="C19" s="66" t="s">
-        <v>1935</v>
-      </c>
-      <c r="D19" s="65" t="s">
-        <v>1923</v>
-      </c>
-      <c r="E19" s="67"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="65" t="s">
-        <v>1936</v>
-      </c>
-      <c r="B20" s="65" t="s">
-        <v>1937</v>
-      </c>
-      <c r="C20" s="66">
-        <v>2</v>
-      </c>
-      <c r="D20" s="65" t="s">
-        <v>1886</v>
-      </c>
-      <c r="E20" s="67"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="65" t="s">
-        <v>1938</v>
-      </c>
-      <c r="B21" s="65" t="s">
-        <v>1939</v>
-      </c>
-      <c r="C21" s="66" t="s">
-        <v>1940</v>
-      </c>
-      <c r="D21" s="65"/>
-      <c r="E21" s="67"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="65" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="65" t="s">
+        <v>1952</v>
+      </c>
+      <c r="B33" s="65" t="s">
         <v>1941</v>
       </c>
-      <c r="B22" s="65" t="s">
+      <c r="C33" s="66" t="s">
         <v>1942</v>
       </c>
-      <c r="C22" s="66" t="s">
-        <v>1943</v>
-      </c>
-      <c r="D22" s="65"/>
-      <c r="E22" s="67"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="65" t="s">
-        <v>1944</v>
-      </c>
-      <c r="B23" s="65" t="s">
-        <v>1945</v>
-      </c>
-      <c r="C23" s="66" t="s">
-        <v>1946</v>
-      </c>
-      <c r="D23" s="65"/>
-      <c r="E23" s="67"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="62" t="s">
-        <v>1948</v>
-      </c>
-      <c r="B25" s="63"/>
-      <c r="C25" s="62" t="s">
-        <v>1882</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="65" t="s">
-        <v>1949</v>
-      </c>
-      <c r="B26" s="65" t="s">
-        <v>1884</v>
-      </c>
-      <c r="C26" s="66" t="s">
-        <v>1885</v>
-      </c>
-      <c r="D26" s="65" t="s">
-        <v>1886</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="65" t="s">
-        <v>1950</v>
-      </c>
-      <c r="B27" s="65" t="s">
-        <v>1888</v>
-      </c>
-      <c r="C27" s="66" t="s">
-        <v>1951</v>
-      </c>
-      <c r="D27" s="65" t="s">
-        <v>1947</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="65" t="s">
-        <v>1952</v>
-      </c>
-      <c r="B28" s="65" t="s">
-        <v>1891</v>
-      </c>
-      <c r="C28" s="66" t="s">
-        <v>1892</v>
-      </c>
-      <c r="D28" s="65" t="s">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="65" t="s">
-        <v>1953</v>
-      </c>
-      <c r="B29" s="65" t="s">
-        <v>1895</v>
-      </c>
-      <c r="C29" s="66" t="s">
-        <v>1896</v>
-      </c>
-      <c r="D29" s="65" t="s">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="65" t="s">
-        <v>1954</v>
-      </c>
-      <c r="B30" s="65" t="s">
-        <v>1955</v>
-      </c>
-      <c r="C30" s="66" t="s">
-        <v>1899</v>
-      </c>
-      <c r="D30" s="65" t="s">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="65" t="s">
-        <v>1956</v>
-      </c>
-      <c r="B31" s="65" t="s">
-        <v>1925</v>
-      </c>
-      <c r="C31" s="66" t="s">
-        <v>1926</v>
-      </c>
-      <c r="D31" s="65" t="s">
-        <v>1886</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="65" t="s">
-        <v>1957</v>
-      </c>
-      <c r="B32" s="65" t="s">
-        <v>1945</v>
-      </c>
-      <c r="C32" s="66" t="s">
-        <v>1946</v>
-      </c>
-      <c r="D32" s="65"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Use the proper mapping spreadsheet and change the name of donorIdentifier to donationIdentificationNumber.
</commit_message>
<xml_diff>
--- a/input/images/ICSR_Field_Listing_and_FHIR_Mapping.xlsx
+++ b/input/images/ICSR_Field_Listing_and_FHIR_Mapping.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeanduteau/Documents/DDIWork/IBM-BEST/fhir-icsr-ae-reporting/input/images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shobbi/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C977DEC0-74B7-F443-AA40-4F1E1F86FD09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4B27BB-F18B-5648-AE16-1D04EA316E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11100" yWindow="28800" windowWidth="26780" windowHeight="19420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11100" yWindow="22100" windowWidth="26780" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICSR FIELDS" sheetId="1" r:id="rId1"/>
-    <sheet name="CASE NARRATIVE FIELDS" sheetId="10" r:id="rId2"/>
-    <sheet name="FAERS FHIR MAPPING" sheetId="8" r:id="rId3"/>
-    <sheet name="VAERS FHIR MAPPING" sheetId="9" r:id="rId4"/>
+    <sheet name="FAERS FHIR MAPPING" sheetId="8" r:id="rId2"/>
+    <sheet name="VAERS FHIR MAPPING" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6511" uniqueCount="1955">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6424" uniqueCount="1881">
   <si>
     <t>CONF</t>
   </si>
@@ -5968,234 +5967,12 @@
   <si>
     <t>processing.procedure</t>
   </si>
-  <si>
-    <t>B.5.1 CASE NARRATIVE RETURN DELIMITED LINES</t>
-  </si>
-  <si>
-    <t>Concatenate description + ": " + value into line</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 1</t>
-  </si>
-  <si>
-    <t>Header:</t>
-  </si>
-  <si>
-    <t>FDA CBER BEST Automated AE Reporting Prototype Case</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 2</t>
-  </si>
-  <si>
-    <t>BEST Detection Phenotype Algorithm:</t>
-  </si>
-  <si>
-    <t>TACO phenotype algorithm (Phenotype Card Link)</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 3</t>
-  </si>
-  <si>
-    <t>BEST Certainty:</t>
-  </si>
-  <si>
-    <t>Definitive</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 4</t>
-  </si>
-  <si>
-    <t>BEST Severity:</t>
-  </si>
-  <si>
-    <t>Severe</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 5</t>
-  </si>
-  <si>
-    <t>BEST Imputability:</t>
-  </si>
-  <si>
-    <t>Probable</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 6</t>
-  </si>
-  <si>
-    <t>Form Type:</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 7</t>
-  </si>
-  <si>
-    <t>Contact Method:</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 8</t>
-  </si>
-  <si>
-    <t>Adverse Event:</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 9</t>
-  </si>
-  <si>
-    <t>Center to which case is being routed to:</t>
-  </si>
-  <si>
-    <t>CBER</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 10</t>
-  </si>
-  <si>
-    <t>Whether the case is being sent to DQRS:</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 11</t>
-  </si>
-  <si>
-    <t>Whether the report is related to drugs or food/cosmetics:</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 12</t>
-  </si>
-  <si>
-    <t>Whether the blood report is of type Transfusion or Collection:</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 13</t>
-  </si>
-  <si>
-    <t>Patient Race Code:</t>
-  </si>
-  <si>
-    <t>&lt;RACE CODE&gt;</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 14</t>
-  </si>
-  <si>
-    <t>Blood group of patient:</t>
-  </si>
-  <si>
-    <t>&lt;PATIENT BLOOD GROUP&gt;</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 15</t>
-  </si>
-  <si>
-    <t>Onset location for reaction:</t>
-  </si>
-  <si>
-    <t>Medstar Location</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 16</t>
-  </si>
-  <si>
-    <t>Description code for blood products:</t>
-  </si>
-  <si>
-    <t>&lt;ISBT-128 CODE&gt;</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 17</t>
-  </si>
-  <si>
-    <t>Blood group and type:</t>
-  </si>
-  <si>
-    <t>&lt;TRANSFUSION BLOOD GROUP/TYPE&gt;</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 18</t>
-  </si>
-  <si>
-    <t>Blood processing type:</t>
-  </si>
-  <si>
-    <t>&lt;ISBT CATEGORY&gt;</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 19</t>
-  </si>
-  <si>
-    <t>Product available for evalution:</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 20</t>
-  </si>
-  <si>
-    <t>Volume of transfusion:</t>
-  </si>
-  <si>
-    <t>&lt;UNITS TRANSFUSED&gt;</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 21</t>
-  </si>
-  <si>
-    <t>NHSN Workup:</t>
-  </si>
-  <si>
-    <t>&lt;INSERT NHSN HEMOVIGILANCE INFORMATION&gt;</t>
-  </si>
-  <si>
-    <t>B.5.1 LINE 22</t>
-  </si>
-  <si>
-    <t>Preliminary investigation results:</t>
-  </si>
-  <si>
-    <t>&lt;INSERT BEST CLINICAL REVIEWER CASE NARRATIVE&gt;</t>
-  </si>
-  <si>
-    <t>H.1 CASE NARRATIVE RETURN DELIMITED LINES</t>
-  </si>
-  <si>
-    <t>H.1 LINE 1</t>
-  </si>
-  <si>
-    <t>H.1 LINE 2</t>
-  </si>
-  <si>
-    <t>Case detected using &lt;OutcomeOfInterest&gt; phenotype algorithm (Phenotype Card Link)</t>
-  </si>
-  <si>
-    <t>H.1 LINE 3</t>
-  </si>
-  <si>
-    <t>H.1 LINE 4</t>
-  </si>
-  <si>
-    <t>H.1 LINE 5</t>
-  </si>
-  <si>
-    <t>BEST Causality:</t>
-  </si>
-  <si>
-    <t>H.1 LINE 6</t>
-  </si>
-  <si>
-    <t>H.1 LINE 7</t>
-  </si>
-  <si>
-    <t>CASE NARRATIVE FIELD</t>
-  </si>
-  <si>
-    <t>SAMPLE DATA</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6263,15 +6040,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6293,12 +6063,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFCE4D6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6331,7 +6095,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -6482,20 +6246,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -6719,7 +6469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1107"/>
   <sheetViews>
-    <sheetView topLeftCell="F243" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -6743,22 +6493,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="62" t="s">
         <v>1741</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="69" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="63" t="s">
         <v>1746</v>
       </c>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -26098,398 +25848,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64062B5B-6E9E-B649-A773-97A21E2861DA}">
-  <dimension ref="A1:D33"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>1953</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1954</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="62" t="s">
-        <v>1881</v>
-      </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="62" t="s">
-        <v>1882</v>
-      </c>
-      <c r="D2" s="64"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="65" t="s">
-        <v>1883</v>
-      </c>
-      <c r="B3" s="65" t="s">
-        <v>1884</v>
-      </c>
-      <c r="C3" s="66" t="s">
-        <v>1885</v>
-      </c>
-      <c r="D3" s="67"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="65" t="s">
-        <v>1886</v>
-      </c>
-      <c r="B4" s="65" t="s">
-        <v>1887</v>
-      </c>
-      <c r="C4" s="66" t="s">
-        <v>1888</v>
-      </c>
-      <c r="D4" s="67"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="65" t="s">
-        <v>1889</v>
-      </c>
-      <c r="B5" s="65" t="s">
-        <v>1890</v>
-      </c>
-      <c r="C5" s="66" t="s">
-        <v>1891</v>
-      </c>
-      <c r="D5" s="67"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="65" t="s">
-        <v>1892</v>
-      </c>
-      <c r="B6" s="65" t="s">
-        <v>1893</v>
-      </c>
-      <c r="C6" s="66" t="s">
-        <v>1894</v>
-      </c>
-      <c r="D6" s="67"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="65" t="s">
-        <v>1895</v>
-      </c>
-      <c r="B7" s="65" t="s">
-        <v>1896</v>
-      </c>
-      <c r="C7" s="66" t="s">
-        <v>1897</v>
-      </c>
-      <c r="D7" s="67"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="65" t="s">
-        <v>1898</v>
-      </c>
-      <c r="B8" s="65" t="s">
-        <v>1899</v>
-      </c>
-      <c r="C8" s="66">
-        <v>3500</v>
-      </c>
-      <c r="D8" s="67"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="65" t="s">
-        <v>1900</v>
-      </c>
-      <c r="B9" s="65" t="s">
-        <v>1901</v>
-      </c>
-      <c r="C9" s="66" t="s">
-        <v>1902</v>
-      </c>
-      <c r="D9" s="67"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="65" t="s">
-        <v>1903</v>
-      </c>
-      <c r="B10" s="65" t="s">
-        <v>1904</v>
-      </c>
-      <c r="C10" s="66">
-        <v>1</v>
-      </c>
-      <c r="D10" s="67"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="65" t="s">
-        <v>1905</v>
-      </c>
-      <c r="B11" s="65" t="s">
-        <v>1906</v>
-      </c>
-      <c r="C11" s="66" t="s">
-        <v>1907</v>
-      </c>
-      <c r="D11" s="67"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="65" t="s">
-        <v>1908</v>
-      </c>
-      <c r="B12" s="65" t="s">
-        <v>1909</v>
-      </c>
-      <c r="C12" s="66" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="67"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="65" t="s">
-        <v>1910</v>
-      </c>
-      <c r="B13" s="65" t="s">
-        <v>1911</v>
-      </c>
-      <c r="C13" s="66">
-        <v>1</v>
-      </c>
-      <c r="D13" s="67"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="65" t="s">
-        <v>1912</v>
-      </c>
-      <c r="B14" s="65" t="s">
-        <v>1913</v>
-      </c>
-      <c r="C14" s="66">
-        <v>2</v>
-      </c>
-      <c r="D14" s="67"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="65" t="s">
-        <v>1914</v>
-      </c>
-      <c r="B15" s="65" t="s">
-        <v>1915</v>
-      </c>
-      <c r="C15" s="66" t="s">
-        <v>1916</v>
-      </c>
-      <c r="D15" s="67"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="65" t="s">
-        <v>1917</v>
-      </c>
-      <c r="B16" s="65" t="s">
-        <v>1918</v>
-      </c>
-      <c r="C16" s="66" t="s">
-        <v>1919</v>
-      </c>
-      <c r="D16" s="67"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="65" t="s">
-        <v>1920</v>
-      </c>
-      <c r="B17" s="65" t="s">
-        <v>1921</v>
-      </c>
-      <c r="C17" s="66" t="s">
-        <v>1922</v>
-      </c>
-      <c r="D17" s="67"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="65" t="s">
-        <v>1923</v>
-      </c>
-      <c r="B18" s="65" t="s">
-        <v>1924</v>
-      </c>
-      <c r="C18" s="66" t="s">
-        <v>1925</v>
-      </c>
-      <c r="D18" s="67"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="65" t="s">
-        <v>1926</v>
-      </c>
-      <c r="B19" s="65" t="s">
-        <v>1927</v>
-      </c>
-      <c r="C19" s="66" t="s">
-        <v>1928</v>
-      </c>
-      <c r="D19" s="67"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="65" t="s">
-        <v>1929</v>
-      </c>
-      <c r="B20" s="65" t="s">
-        <v>1930</v>
-      </c>
-      <c r="C20" s="66" t="s">
-        <v>1931</v>
-      </c>
-      <c r="D20" s="67"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="65" t="s">
-        <v>1932</v>
-      </c>
-      <c r="B21" s="65" t="s">
-        <v>1933</v>
-      </c>
-      <c r="C21" s="66">
-        <v>2</v>
-      </c>
-      <c r="D21" s="67"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="65" t="s">
-        <v>1934</v>
-      </c>
-      <c r="B22" s="65" t="s">
-        <v>1935</v>
-      </c>
-      <c r="C22" s="66" t="s">
-        <v>1936</v>
-      </c>
-      <c r="D22" s="67"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="65" t="s">
-        <v>1937</v>
-      </c>
-      <c r="B23" s="65" t="s">
-        <v>1938</v>
-      </c>
-      <c r="C23" s="66" t="s">
-        <v>1939</v>
-      </c>
-      <c r="D23" s="67"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="65" t="s">
-        <v>1940</v>
-      </c>
-      <c r="B24" s="65" t="s">
-        <v>1941</v>
-      </c>
-      <c r="C24" s="66" t="s">
-        <v>1942</v>
-      </c>
-      <c r="D24" s="67"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="62" t="s">
-        <v>1943</v>
-      </c>
-      <c r="B26" s="63"/>
-      <c r="C26" s="62" t="s">
-        <v>1882</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="65" t="s">
-        <v>1944</v>
-      </c>
-      <c r="B27" s="65" t="s">
-        <v>1884</v>
-      </c>
-      <c r="C27" s="66" t="s">
-        <v>1885</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="65" t="s">
-        <v>1945</v>
-      </c>
-      <c r="B28" s="65" t="s">
-        <v>1887</v>
-      </c>
-      <c r="C28" s="66" t="s">
-        <v>1946</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="65" t="s">
-        <v>1947</v>
-      </c>
-      <c r="B29" s="65" t="s">
-        <v>1890</v>
-      </c>
-      <c r="C29" s="66" t="s">
-        <v>1891</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="65" t="s">
-        <v>1948</v>
-      </c>
-      <c r="B30" s="65" t="s">
-        <v>1893</v>
-      </c>
-      <c r="C30" s="66" t="s">
-        <v>1894</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="65" t="s">
-        <v>1949</v>
-      </c>
-      <c r="B31" s="65" t="s">
-        <v>1950</v>
-      </c>
-      <c r="C31" s="66" t="s">
-        <v>1897</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="65" t="s">
-        <v>1951</v>
-      </c>
-      <c r="B32" s="65" t="s">
-        <v>1921</v>
-      </c>
-      <c r="C32" s="66" t="s">
-        <v>1922</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="65" t="s">
-        <v>1952</v>
-      </c>
-      <c r="B33" s="65" t="s">
-        <v>1941</v>
-      </c>
-      <c r="C33" s="66" t="s">
-        <v>1942</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFDF31D-DB87-5B44-A82D-620975583361}">
   <dimension ref="A1:I555"/>
   <sheetViews>
-    <sheetView topLeftCell="A497" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
@@ -32816,7 +32178,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3776FE-6EB3-844A-B62D-00DDF92F1B48}">
   <dimension ref="A1:J697"/>
   <sheetViews>

</xml_diff>